<commit_message>
Added content to README
</commit_message>
<xml_diff>
--- a/test/data/two_sheets.xlsx
+++ b/test/data/two_sheets.xlsx
@@ -4,11 +4,11 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Лист1"/>
-    <sheet r:id="rId2" sheetId="2" name="Лист2"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet r:id="rId2" sheetId="2" name="Sheet2"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
@@ -85,7 +85,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -107,9 +107,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -415,11 +412,11 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
@@ -483,17 +480,17 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="15.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -503,7 +500,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="15.75">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -513,7 +510,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="15.75">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -523,7 +520,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="15.75">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -533,7 +530,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="15.75">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -545,7 +542,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="15.75">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -557,7 +554,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="15.75">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="5">
@@ -565,7 +562,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="15.75">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="1"/>

</xml_diff>